<commit_message>
Update database layer and unit testcases
</commit_message>
<xml_diff>
--- a/testExcelFiles/testRules.xlsx
+++ b/testExcelFiles/testRules.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="test_rules" sheetId="1" r:id="rId1"/>
-    <sheet name="gender_rules" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,30 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>month</t>
   </si>
   <si>
     <t>quarter</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>Josh</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Wendy</t>
-  </si>
-  <si>
-    <t>Female</t>
   </si>
 </sst>
 </file>
@@ -363,8 +344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,43 +457,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>